<commit_message>
updated tanzania data to be able to run
</commit_message>
<xml_diff>
--- a/article_6_tanzania_sri_lanka_peru/transformations/templates/calibrated/sri_lanka/model_input_variables_sri_lanka_ip_calibrated.xlsx
+++ b/article_6_tanzania_sri_lanka_peru/transformations/templates/calibrated/sri_lanka/model_input_variables_sri_lanka_ip_calibrated.xlsx
@@ -12847,112 +12847,112 @@
         <v>1</v>
       </c>
       <c r="J97">
-        <v>0.056947487651181</v>
+        <v>7.352557421706344</v>
       </c>
       <c r="K97">
-        <v>0.056947487651181</v>
+        <v>-3.373132943588593</v>
       </c>
       <c r="L97">
-        <v>0.056947487651181</v>
+        <v>-6.488892781360207</v>
       </c>
       <c r="M97">
-        <v>0.056947487651181</v>
+        <v>0.1138069291024017</v>
       </c>
       <c r="N97">
-        <v>0.056947487651181</v>
+        <v>4.227970163916579</v>
       </c>
       <c r="O97">
-        <v>0.056947487651181</v>
+        <v>0</v>
       </c>
       <c r="P97">
-        <v>0.056947487651181</v>
+        <v>0.0333333333333333</v>
       </c>
       <c r="Q97">
-        <v>0.056947487651181</v>
+        <v>0.0666666666666666</v>
       </c>
       <c r="R97">
-        <v>0.056947487651181</v>
+        <v>0.1</v>
       </c>
       <c r="S97">
-        <v>0.056947487651181</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="T97">
-        <v>0.056947487651181</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="U97">
-        <v>0.056947487651181</v>
+        <v>0.2</v>
       </c>
       <c r="V97">
-        <v>0.056947487651181</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="W97">
-        <v>0.056947487651181</v>
+        <v>0.2666666666666666</v>
       </c>
       <c r="X97">
-        <v>0.056947487651181</v>
+        <v>0.3</v>
       </c>
       <c r="Y97">
-        <v>0.056947487651181</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="Z97">
-        <v>0.056947487651181</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="AA97">
-        <v>0.0569474876511811</v>
+        <v>0.4</v>
       </c>
       <c r="AB97">
-        <v>0.0569474876511811</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="AC97">
-        <v>0.0569474876511811</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="AD97">
-        <v>0.0569474876511811</v>
+        <v>0.5</v>
       </c>
       <c r="AE97">
-        <v>0.0569474876511811</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="AF97">
-        <v>0.0569474876511811</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="AG97">
-        <v>0.0569474876511811</v>
+        <v>0.6</v>
       </c>
       <c r="AH97">
-        <v>0.0569474876511811</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="AI97">
-        <v>0.0569474876511811</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AJ97">
-        <v>0.0569474876511811</v>
+        <v>0.7</v>
       </c>
       <c r="AK97">
-        <v>0.0569474876511811</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="AL97">
-        <v>0.0569474876511811</v>
+        <v>0.7666666666666666</v>
       </c>
       <c r="AM97">
-        <v>0.0569474876511811</v>
+        <v>0.8</v>
       </c>
       <c r="AN97">
-        <v>0.0569474876511811</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AO97">
-        <v>0.0569474876511811</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AP97">
-        <v>0.0569474876511811</v>
+        <v>0.9</v>
       </c>
       <c r="AQ97">
-        <v>0.0569474876511811</v>
+        <v>0.9333333333333332</v>
       </c>
       <c r="AR97">
-        <v>0.0569474876511811</v>
+        <v>0.9666666666666668</v>
       </c>
       <c r="AS97">
-        <v>0.0569474876511811</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:45">
@@ -12969,112 +12969,112 @@
         <v>1</v>
       </c>
       <c r="J98">
-        <v>0.109927728802231</v>
+        <v>-7.778556027190428</v>
       </c>
       <c r="K98">
-        <v>0.109927728802231</v>
+        <v>0.9027260209021361</v>
       </c>
       <c r="L98">
-        <v>0.109927728802231</v>
+        <v>1.048935941166182</v>
       </c>
       <c r="M98">
-        <v>0.109927728802231</v>
+        <v>1.383862547128134</v>
       </c>
       <c r="N98">
-        <v>0.109927728802231</v>
+        <v>-2.316354931466868</v>
       </c>
       <c r="O98">
-        <v>0.109927728802231</v>
+        <v>0</v>
       </c>
       <c r="P98">
-        <v>0.109927728802231</v>
+        <v>0.0333333333333333</v>
       </c>
       <c r="Q98">
-        <v>0.109927728802231</v>
+        <v>0.0666666666666666</v>
       </c>
       <c r="R98">
-        <v>0.109927728802231</v>
+        <v>0.1</v>
       </c>
       <c r="S98">
-        <v>0.109927728802231</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="T98">
-        <v>0.109927728802231</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="U98">
-        <v>0.109927728802231</v>
+        <v>0.2</v>
       </c>
       <c r="V98">
-        <v>0.109927728802231</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="W98">
-        <v>0.109927728802231</v>
+        <v>0.2666666666666666</v>
       </c>
       <c r="X98">
-        <v>0.109927728802231</v>
+        <v>0.3</v>
       </c>
       <c r="Y98">
-        <v>0.109927728802231</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="Z98">
-        <v>0.109927728802231</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="AA98">
-        <v>0.109927728802232</v>
+        <v>0.4</v>
       </c>
       <c r="AB98">
-        <v>0.109927728802232</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="AC98">
-        <v>0.109927728802232</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="AD98">
-        <v>0.109927728802232</v>
+        <v>0.5</v>
       </c>
       <c r="AE98">
-        <v>0.109927728802232</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="AF98">
-        <v>0.109927728802232</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="AG98">
-        <v>0.109927728802232</v>
+        <v>0.6</v>
       </c>
       <c r="AH98">
-        <v>0.109927728802232</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="AI98">
-        <v>0.109927728802232</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AJ98">
-        <v>0.109927728802232</v>
+        <v>0.7</v>
       </c>
       <c r="AK98">
-        <v>0.109927728802232</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="AL98">
-        <v>0.109927728802232</v>
+        <v>0.7666666666666666</v>
       </c>
       <c r="AM98">
-        <v>0.109927728802232</v>
+        <v>0.8</v>
       </c>
       <c r="AN98">
-        <v>0.109927728802232</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AO98">
-        <v>0.109927728802232</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AP98">
-        <v>0.109927728802232</v>
+        <v>0.9</v>
       </c>
       <c r="AQ98">
-        <v>0.109927728802232</v>
+        <v>0.9333333333333332</v>
       </c>
       <c r="AR98">
-        <v>0.109927728802232</v>
+        <v>0.9666666666666668</v>
       </c>
       <c r="AS98">
-        <v>0.109927728802232</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:45">
@@ -13091,112 +13091,112 @@
         <v>1</v>
       </c>
       <c r="J99">
-        <v>0.0467616205881656</v>
+        <v>4.498888620842355</v>
       </c>
       <c r="K99">
-        <v>0.0467616205881656</v>
+        <v>1.264092425302407</v>
       </c>
       <c r="L99">
-        <v>0.0467616205881656</v>
+        <v>-0.0109603687084165</v>
       </c>
       <c r="M99">
-        <v>0.0467616205881656</v>
+        <v>0.7291214146152644</v>
       </c>
       <c r="N99">
-        <v>0.0467616205881656</v>
+        <v>-1.261182291616252</v>
       </c>
       <c r="O99">
-        <v>0.0467616205881656</v>
+        <v>0</v>
       </c>
       <c r="P99">
-        <v>0.0467616205881656</v>
+        <v>0.0333333333333333</v>
       </c>
       <c r="Q99">
-        <v>0.0467616205881656</v>
+        <v>0.0666666666666666</v>
       </c>
       <c r="R99">
-        <v>0.0467616205881656</v>
+        <v>0.1</v>
       </c>
       <c r="S99">
-        <v>0.0467616205881656</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="T99">
-        <v>0.0467616205881656</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="U99">
-        <v>0.0467616205881656</v>
+        <v>0.2</v>
       </c>
       <c r="V99">
-        <v>0.0467616205881656</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="W99">
-        <v>0.0467616205881656</v>
+        <v>0.2666666666666666</v>
       </c>
       <c r="X99">
-        <v>0.0467616205881656</v>
+        <v>0.3</v>
       </c>
       <c r="Y99">
-        <v>0.0467616205881656</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="Z99">
-        <v>0.0467616205881656</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="AA99">
-        <v>0.0467616205881656</v>
+        <v>0.4</v>
       </c>
       <c r="AB99">
-        <v>0.0467616205881656</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="AC99">
-        <v>0.0467616205881656</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="AD99">
-        <v>0.0467616205881656</v>
+        <v>0.5</v>
       </c>
       <c r="AE99">
-        <v>0.0467616205881656</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="AF99">
-        <v>0.0467616205881656</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="AG99">
-        <v>0.0467616205881656</v>
+        <v>0.6</v>
       </c>
       <c r="AH99">
-        <v>0.0467616205881656</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="AI99">
-        <v>0.0467616205881656</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AJ99">
-        <v>0.0467616205881656</v>
+        <v>0.7</v>
       </c>
       <c r="AK99">
-        <v>0.0467616205881656</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="AL99">
-        <v>0.0467616205881656</v>
+        <v>0.7666666666666666</v>
       </c>
       <c r="AM99">
-        <v>0.0467616205881656</v>
+        <v>0.8</v>
       </c>
       <c r="AN99">
-        <v>0.0467616205881656</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AO99">
-        <v>0.0467616205881656</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AP99">
-        <v>0.0467616205881656</v>
+        <v>0.9</v>
       </c>
       <c r="AQ99">
-        <v>0.0467616205881656</v>
+        <v>0.9333333333333332</v>
       </c>
       <c r="AR99">
-        <v>0.0467616205881656</v>
+        <v>0.9666666666666668</v>
       </c>
       <c r="AS99">
-        <v>0.0467616205881656</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:45">
@@ -13213,112 +13213,112 @@
         <v>1</v>
       </c>
       <c r="J100">
-        <v>0.0406843818147015</v>
+        <v>-2.881501143613087</v>
       </c>
       <c r="K100">
-        <v>0.0406843818147015</v>
+        <v>-0.2968302677760844</v>
       </c>
       <c r="L100">
-        <v>0.0406843818147015</v>
+        <v>0.387496673938261</v>
       </c>
       <c r="M100">
-        <v>0.0406843818147015</v>
+        <v>-4.423440663835002</v>
       </c>
       <c r="N100">
-        <v>0.0406843818147015</v>
+        <v>3.448999547701408</v>
       </c>
       <c r="O100">
-        <v>0.0406843818147015</v>
+        <v>0</v>
       </c>
       <c r="P100">
-        <v>0.0406843818147015</v>
+        <v>0.0333333333333333</v>
       </c>
       <c r="Q100">
-        <v>0.0406843818147015</v>
+        <v>0.0666666666666666</v>
       </c>
       <c r="R100">
-        <v>0.0406843818147015</v>
+        <v>0.1</v>
       </c>
       <c r="S100">
-        <v>0.0406843818147015</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="T100">
-        <v>0.0406843818147015</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="U100">
-        <v>0.0406843818147015</v>
+        <v>0.2</v>
       </c>
       <c r="V100">
-        <v>0.0406843818147015</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="W100">
-        <v>0.0406843818147015</v>
+        <v>0.2666666666666666</v>
       </c>
       <c r="X100">
-        <v>0.0406843818147015</v>
+        <v>0.3</v>
       </c>
       <c r="Y100">
-        <v>0.0406843818147015</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="Z100">
-        <v>0.0406843818147015</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="AA100">
-        <v>0.0406843818147016</v>
+        <v>0.4</v>
       </c>
       <c r="AB100">
-        <v>0.0406843818147016</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="AC100">
-        <v>0.0406843818147016</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="AD100">
-        <v>0.0406843818147016</v>
+        <v>0.5</v>
       </c>
       <c r="AE100">
-        <v>0.0406843818147016</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="AF100">
-        <v>0.0406843818147016</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="AG100">
-        <v>0.0406843818147016</v>
+        <v>0.6</v>
       </c>
       <c r="AH100">
-        <v>0.0406843818147016</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="AI100">
-        <v>0.0406843818147016</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AJ100">
-        <v>0.0406843818147016</v>
+        <v>0.7</v>
       </c>
       <c r="AK100">
-        <v>0.0406843818147016</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="AL100">
-        <v>0.0406843818147016</v>
+        <v>0.7666666666666666</v>
       </c>
       <c r="AM100">
-        <v>0.0406843818147016</v>
+        <v>0.8</v>
       </c>
       <c r="AN100">
-        <v>0.0406843818147016</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AO100">
-        <v>0.0406843818147016</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AP100">
-        <v>0.0406843818147016</v>
+        <v>0.9</v>
       </c>
       <c r="AQ100">
-        <v>0.0406843818147016</v>
+        <v>0.9333333333333332</v>
       </c>
       <c r="AR100">
-        <v>0.0406843818147016</v>
+        <v>0.9666666666666668</v>
       </c>
       <c r="AS100">
-        <v>0.0406843818147016</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:45">
@@ -13335,112 +13335,112 @@
         <v>1</v>
       </c>
       <c r="J101">
-        <v>0.0240312533986499</v>
+        <v>0.2751575730778546</v>
       </c>
       <c r="K101">
-        <v>0.0240312533986499</v>
+        <v>22.09430693376326</v>
       </c>
       <c r="L101">
-        <v>0.0240312533986499</v>
+        <v>-13.45110173287774</v>
       </c>
       <c r="M101">
-        <v>0.0240312533986499</v>
+        <v>-9.545530866041863</v>
       </c>
       <c r="N101">
-        <v>0.0240312533986499</v>
+        <v>26.97708393610572</v>
       </c>
       <c r="O101">
-        <v>0.0240312533986499</v>
+        <v>0</v>
       </c>
       <c r="P101">
-        <v>0.0240312533986499</v>
+        <v>0.0333333333333333</v>
       </c>
       <c r="Q101">
-        <v>0.0240312533986499</v>
+        <v>0.0666666666666666</v>
       </c>
       <c r="R101">
-        <v>0.0240312533986499</v>
+        <v>0.1</v>
       </c>
       <c r="S101">
-        <v>0.0240312533986499</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="T101">
-        <v>0.0240312533986499</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="U101">
-        <v>0.0240312533986499</v>
+        <v>0.2</v>
       </c>
       <c r="V101">
-        <v>0.0240312533986499</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="W101">
-        <v>0.0240312533986499</v>
+        <v>0.2666666666666666</v>
       </c>
       <c r="X101">
-        <v>0.0240312533986499</v>
+        <v>0.3</v>
       </c>
       <c r="Y101">
-        <v>0.0240312533986499</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="Z101">
-        <v>0.0240312533986499</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="AA101">
-        <v>0.02403125339865</v>
+        <v>0.4</v>
       </c>
       <c r="AB101">
-        <v>0.02403125339865</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="AC101">
-        <v>0.02403125339865</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="AD101">
-        <v>0.02403125339865</v>
+        <v>0.5</v>
       </c>
       <c r="AE101">
-        <v>0.02403125339865</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="AF101">
-        <v>0.02403125339865</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="AG101">
-        <v>0.02403125339865</v>
+        <v>0.6</v>
       </c>
       <c r="AH101">
-        <v>0.02403125339865</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="AI101">
-        <v>0.02403125339865</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AJ101">
-        <v>0.02403125339865</v>
+        <v>0.7</v>
       </c>
       <c r="AK101">
-        <v>0.02403125339865</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="AL101">
-        <v>0.02403125339865</v>
+        <v>0.7666666666666666</v>
       </c>
       <c r="AM101">
-        <v>0.02403125339865</v>
+        <v>0.8</v>
       </c>
       <c r="AN101">
-        <v>0.02403125339865</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AO101">
-        <v>0.02403125339865</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AP101">
-        <v>0.02403125339865</v>
+        <v>0.9</v>
       </c>
       <c r="AQ101">
-        <v>0.02403125339865</v>
+        <v>0.9333333333333332</v>
       </c>
       <c r="AR101">
-        <v>0.02403125339865</v>
+        <v>0.9666666666666668</v>
       </c>
       <c r="AS101">
-        <v>0.02403125339865</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:45">
@@ -13457,112 +13457,112 @@
         <v>1</v>
       </c>
       <c r="J102">
-        <v>0.0461351747938064</v>
+        <v>5.763545076972254</v>
       </c>
       <c r="K102">
-        <v>0.0461351747938064</v>
+        <v>1.107057815380003</v>
       </c>
       <c r="L102">
-        <v>0.0461351747938064</v>
+        <v>-3.775154178420026</v>
       </c>
       <c r="M102">
-        <v>0.0461351747938064</v>
+        <v>5.816744542977935</v>
       </c>
       <c r="N102">
-        <v>0.0461351747938064</v>
+        <v>-2.77803372183387</v>
       </c>
       <c r="O102">
-        <v>0.0461351747938064</v>
+        <v>0</v>
       </c>
       <c r="P102">
-        <v>0.0461351747938064</v>
+        <v>0.0333333333333333</v>
       </c>
       <c r="Q102">
-        <v>0.0461351747938064</v>
+        <v>0.0666666666666666</v>
       </c>
       <c r="R102">
-        <v>0.0461351747938064</v>
+        <v>0.1</v>
       </c>
       <c r="S102">
-        <v>0.0461351747938064</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="T102">
-        <v>0.0461351747938064</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="U102">
-        <v>0.0461351747938064</v>
+        <v>0.2</v>
       </c>
       <c r="V102">
-        <v>0.0461351747938064</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="W102">
-        <v>0.0461351747938064</v>
+        <v>0.2666666666666666</v>
       </c>
       <c r="X102">
-        <v>0.0461351747938064</v>
+        <v>0.3</v>
       </c>
       <c r="Y102">
-        <v>0.0461351747938064</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="Z102">
-        <v>0.0461351747938064</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="AA102">
-        <v>0.0461351747938064</v>
+        <v>0.4</v>
       </c>
       <c r="AB102">
-        <v>0.0461351747938064</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="AC102">
-        <v>0.0461351747938064</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="AD102">
-        <v>0.0461351747938064</v>
+        <v>0.5</v>
       </c>
       <c r="AE102">
-        <v>0.0461351747938064</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="AF102">
-        <v>0.0461351747938064</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="AG102">
-        <v>0.0461351747938064</v>
+        <v>0.6</v>
       </c>
       <c r="AH102">
-        <v>0.0461351747938064</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="AI102">
-        <v>0.0461351747938064</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AJ102">
-        <v>0.0461351747938064</v>
+        <v>0.7</v>
       </c>
       <c r="AK102">
-        <v>0.0461351747938064</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="AL102">
-        <v>0.0461351747938064</v>
+        <v>0.7666666666666666</v>
       </c>
       <c r="AM102">
-        <v>0.0461351747938064</v>
+        <v>0.8</v>
       </c>
       <c r="AN102">
-        <v>0.0461351747938064</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AO102">
-        <v>0.0461351747938064</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AP102">
-        <v>0.0461351747938064</v>
+        <v>0.9</v>
       </c>
       <c r="AQ102">
-        <v>0.0461351747938064</v>
+        <v>0.9333333333333332</v>
       </c>
       <c r="AR102">
-        <v>0.0461351747938064</v>
+        <v>0.9666666666666668</v>
       </c>
       <c r="AS102">
-        <v>0.0461351747938064</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:45">
@@ -13579,112 +13579,112 @@
         <v>1</v>
       </c>
       <c r="J103">
-        <v>0.5</v>
+        <v>-10.22911202776086</v>
       </c>
       <c r="K103">
-        <v>0.5</v>
+        <v>-0.2945226864701558</v>
       </c>
       <c r="L103">
-        <v>0.5</v>
+        <v>1.872952188971701</v>
       </c>
       <c r="M103">
-        <v>0.5</v>
+        <v>1.559552282011421</v>
       </c>
       <c r="N103">
-        <v>0.5</v>
+        <v>-0.2041127431485946</v>
       </c>
       <c r="O103">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P103">
-        <v>0.5</v>
+        <v>0.0333333333333333</v>
       </c>
       <c r="Q103">
-        <v>0.5</v>
+        <v>0.0666666666666666</v>
       </c>
       <c r="R103">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="S103">
-        <v>0.5</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="T103">
-        <v>0.5</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="U103">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="V103">
-        <v>0.5</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="W103">
-        <v>0.5</v>
+        <v>0.2666666666666666</v>
       </c>
       <c r="X103">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="Y103">
-        <v>0.5</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="Z103">
-        <v>0.5</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="AA103">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB103">
-        <v>0.5</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="AC103">
-        <v>0.5</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="AD103">
         <v>0.5</v>
       </c>
       <c r="AE103">
-        <v>0.5</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="AF103">
-        <v>0.5</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="AG103">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="AH103">
-        <v>0.5</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="AI103">
-        <v>0.5</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AJ103">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="AK103">
-        <v>0.5</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="AL103">
-        <v>0.5</v>
+        <v>0.7666666666666666</v>
       </c>
       <c r="AM103">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="AN103">
-        <v>0.5</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AO103">
-        <v>0.5</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AP103">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="AQ103">
-        <v>0.5</v>
+        <v>0.9333333333333332</v>
       </c>
       <c r="AR103">
-        <v>0.5</v>
+        <v>0.9666666666666668</v>
       </c>
       <c r="AS103">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:45">
@@ -13701,112 +13701,112 @@
         <v>1</v>
       </c>
       <c r="J104">
-        <v>0.105163771605354</v>
+        <v>-0.0010643550799541</v>
       </c>
       <c r="K104">
-        <v>0.105163771605354</v>
+        <v>1.3452863035827</v>
       </c>
       <c r="L104">
-        <v>0.105163771605354</v>
+        <v>-1.777287280633069</v>
       </c>
       <c r="M104">
-        <v>0.105163771605354</v>
+        <v>-1.706565729061001</v>
       </c>
       <c r="N104">
-        <v>0.105163771605354</v>
+        <v>1.589989995486501</v>
       </c>
       <c r="O104">
-        <v>0.105163771605354</v>
+        <v>0</v>
       </c>
       <c r="P104">
-        <v>0.105163771605354</v>
+        <v>0.0333333333333333</v>
       </c>
       <c r="Q104">
-        <v>0.105163771605354</v>
+        <v>0.0666666666666666</v>
       </c>
       <c r="R104">
-        <v>0.105163771605354</v>
+        <v>0.1</v>
       </c>
       <c r="S104">
-        <v>0.105163771605354</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="T104">
-        <v>0.105163771605354</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="U104">
-        <v>0.105163771605354</v>
+        <v>0.2</v>
       </c>
       <c r="V104">
-        <v>0.105163771605354</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="W104">
-        <v>0.105163771605354</v>
+        <v>0.2666666666666666</v>
       </c>
       <c r="X104">
-        <v>0.105163771605354</v>
+        <v>0.3</v>
       </c>
       <c r="Y104">
-        <v>0.105163771605354</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="Z104">
-        <v>0.105163771605354</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="AA104">
-        <v>0.105163771605354</v>
+        <v>0.4</v>
       </c>
       <c r="AB104">
-        <v>0.105163771605354</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="AC104">
-        <v>0.105163771605354</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="AD104">
-        <v>0.105163771605354</v>
+        <v>0.5</v>
       </c>
       <c r="AE104">
-        <v>0.105163771605354</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="AF104">
-        <v>0.105163771605354</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="AG104">
-        <v>0.105163771605354</v>
+        <v>0.6</v>
       </c>
       <c r="AH104">
-        <v>0.105163771605354</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="AI104">
-        <v>0.105163771605354</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AJ104">
-        <v>0.105163771605354</v>
+        <v>0.7</v>
       </c>
       <c r="AK104">
-        <v>0.105163771605354</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="AL104">
-        <v>0.105163771605354</v>
+        <v>0.7666666666666666</v>
       </c>
       <c r="AM104">
-        <v>0.105163771605354</v>
+        <v>0.8</v>
       </c>
       <c r="AN104">
-        <v>0.105163771605354</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AO104">
-        <v>0.105163771605354</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AP104">
-        <v>0.105163771605354</v>
+        <v>0.9</v>
       </c>
       <c r="AQ104">
-        <v>0.105163771605354</v>
+        <v>0.9333333333333332</v>
       </c>
       <c r="AR104">
-        <v>0.105163771605354</v>
+        <v>0.9666666666666668</v>
       </c>
       <c r="AS104">
-        <v>0.105163771605354</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:45">
@@ -13823,112 +13823,112 @@
         <v>1</v>
       </c>
       <c r="J105">
-        <v>0.0551216230133952</v>
+        <v>0.8906164334319027</v>
       </c>
       <c r="K105">
-        <v>0.0551216230133952</v>
+        <v>-0.2775917300133474</v>
       </c>
       <c r="L105">
-        <v>0.0551216230133952</v>
+        <v>0.1680711249933744</v>
       </c>
       <c r="M105">
-        <v>0.0551216230133952</v>
+        <v>-1.107515871538016</v>
       </c>
       <c r="N105">
-        <v>0.0551216230133952</v>
+        <v>0.0487905994622913</v>
       </c>
       <c r="O105">
-        <v>0.0551216230133952</v>
+        <v>0</v>
       </c>
       <c r="P105">
-        <v>0.0551216230133952</v>
+        <v>0.0333333333333333</v>
       </c>
       <c r="Q105">
-        <v>0.0551216230133952</v>
+        <v>0.0666666666666666</v>
       </c>
       <c r="R105">
-        <v>0.0551216230133952</v>
+        <v>0.1</v>
       </c>
       <c r="S105">
-        <v>0.0551216230133952</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="T105">
-        <v>0.0551216230133952</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="U105">
-        <v>0.0551216230133952</v>
+        <v>0.2</v>
       </c>
       <c r="V105">
-        <v>0.0551216230133952</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="W105">
-        <v>0.0551216230133952</v>
+        <v>0.2666666666666666</v>
       </c>
       <c r="X105">
-        <v>0.0551216230133952</v>
+        <v>0.3</v>
       </c>
       <c r="Y105">
-        <v>0.0551216230133952</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="Z105">
-        <v>0.0551216230133952</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="AA105">
-        <v>0.0551216230133952</v>
+        <v>0.4</v>
       </c>
       <c r="AB105">
-        <v>0.0551216230133952</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="AC105">
-        <v>0.0551216230133952</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="AD105">
-        <v>0.0551216230133952</v>
+        <v>0.5</v>
       </c>
       <c r="AE105">
-        <v>0.0551216230133952</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="AF105">
-        <v>0.0551216230133952</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="AG105">
-        <v>0.0551216230133952</v>
+        <v>0.6</v>
       </c>
       <c r="AH105">
-        <v>0.0551216230133952</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="AI105">
-        <v>0.0551216230133952</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AJ105">
-        <v>0.0551216230133952</v>
+        <v>0.7</v>
       </c>
       <c r="AK105">
-        <v>0.0551216230133952</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="AL105">
-        <v>0.0551216230133952</v>
+        <v>0.7666666666666666</v>
       </c>
       <c r="AM105">
-        <v>0.0551216230133952</v>
+        <v>0.8</v>
       </c>
       <c r="AN105">
-        <v>0.0551216230133952</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AO105">
-        <v>0.0551216230133952</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AP105">
-        <v>0.0551216230133952</v>
+        <v>0.9</v>
       </c>
       <c r="AQ105">
-        <v>0.0551216230133952</v>
+        <v>0.9333333333333332</v>
       </c>
       <c r="AR105">
-        <v>0.0551216230133952</v>
+        <v>0.9666666666666668</v>
       </c>
       <c r="AS105">
-        <v>0.0551216230133952</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:45">
@@ -14433,112 +14433,112 @@
         <v>1</v>
       </c>
       <c r="J110">
-        <v>0.0133281107617239</v>
+        <v>1.137224907363719</v>
       </c>
       <c r="K110">
-        <v>0.0133281107617239</v>
+        <v>0.4740441610949519</v>
       </c>
       <c r="L110">
-        <v>0.0133281107617239</v>
+        <v>-3.751323708564448</v>
       </c>
       <c r="M110">
-        <v>0.0133281107617239</v>
+        <v>3.232817727912479</v>
       </c>
       <c r="N110">
-        <v>0.0133281107617239</v>
+        <v>-1.65726284174617</v>
       </c>
       <c r="O110">
-        <v>0.0133281107617239</v>
+        <v>0</v>
       </c>
       <c r="P110">
-        <v>0.0133281107617239</v>
+        <v>0.0333333333333333</v>
       </c>
       <c r="Q110">
-        <v>0.0133281107617239</v>
+        <v>0.0666666666666666</v>
       </c>
       <c r="R110">
-        <v>0.0133281107617239</v>
+        <v>0.1</v>
       </c>
       <c r="S110">
-        <v>0.0133281107617239</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="T110">
-        <v>0.0133281107617239</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="U110">
-        <v>0.0133281107617239</v>
+        <v>0.2</v>
       </c>
       <c r="V110">
-        <v>0.0133281107617239</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="W110">
-        <v>0.0133281107617239</v>
+        <v>0.2666666666666666</v>
       </c>
       <c r="X110">
-        <v>0.0133281107617239</v>
+        <v>0.3</v>
       </c>
       <c r="Y110">
-        <v>0.0133281107617239</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="Z110">
-        <v>0.0133281107617239</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="AA110">
-        <v>0.0133281107617239</v>
+        <v>0.4</v>
       </c>
       <c r="AB110">
-        <v>0.0133281107617239</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="AC110">
-        <v>0.0133281107617239</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="AD110">
-        <v>0.0133281107617239</v>
+        <v>0.5</v>
       </c>
       <c r="AE110">
-        <v>0.0133281107617239</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="AF110">
-        <v>0.0133281107617239</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="AG110">
-        <v>0.0133281107617239</v>
+        <v>0.6</v>
       </c>
       <c r="AH110">
-        <v>0.0133281107617239</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="AI110">
-        <v>0.0133281107617239</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AJ110">
-        <v>0.0133281107617239</v>
+        <v>0.7</v>
       </c>
       <c r="AK110">
-        <v>0.0133281107617239</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="AL110">
-        <v>0.0133281107617239</v>
+        <v>0.7666666666666666</v>
       </c>
       <c r="AM110">
-        <v>0.0133281107617239</v>
+        <v>0.8</v>
       </c>
       <c r="AN110">
-        <v>0.0133281107617239</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AO110">
-        <v>0.0133281107617239</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AP110">
-        <v>0.0133281107617239</v>
+        <v>0.9</v>
       </c>
       <c r="AQ110">
-        <v>0.0133281107617239</v>
+        <v>0.9333333333333332</v>
       </c>
       <c r="AR110">
-        <v>0.0133281107617239</v>
+        <v>0.9666666666666668</v>
       </c>
       <c r="AS110">
-        <v>0.0133281107617239</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:45">
@@ -14555,112 +14555,112 @@
         <v>1</v>
       </c>
       <c r="J111">
-        <v>0.0144623715219995</v>
+        <v>2.492445319429683</v>
       </c>
       <c r="K111">
-        <v>0.0144623715219995</v>
+        <v>0.2549311301145209</v>
       </c>
       <c r="L111">
-        <v>0.0144623715219995</v>
+        <v>-5.270166123553977</v>
       </c>
       <c r="M111">
-        <v>0.0144623715219995</v>
+        <v>3.430857869259565</v>
       </c>
       <c r="N111">
-        <v>0.0144623715219995</v>
+        <v>-0.4853753920328891</v>
       </c>
       <c r="O111">
-        <v>0.0144623715219995</v>
+        <v>0</v>
       </c>
       <c r="P111">
-        <v>0.0144623715219995</v>
+        <v>0.0333333333333333</v>
       </c>
       <c r="Q111">
-        <v>0.0144623715219995</v>
+        <v>0.0666666666666666</v>
       </c>
       <c r="R111">
-        <v>0.0144623715219995</v>
+        <v>0.1</v>
       </c>
       <c r="S111">
-        <v>0.0144623715219995</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="T111">
-        <v>0.0144623715219995</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="U111">
-        <v>0.0144623715219995</v>
+        <v>0.2</v>
       </c>
       <c r="V111">
-        <v>0.0144623715219995</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="W111">
-        <v>0.0144623715219995</v>
+        <v>0.2666666666666666</v>
       </c>
       <c r="X111">
-        <v>0.0144623715219995</v>
+        <v>0.3</v>
       </c>
       <c r="Y111">
-        <v>0.0144623715219995</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="Z111">
-        <v>0.0144623715219995</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="AA111">
-        <v>0.0144623715219996</v>
+        <v>0.4</v>
       </c>
       <c r="AB111">
-        <v>0.0144623715219996</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="AC111">
-        <v>0.0144623715219996</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="AD111">
-        <v>0.0144623715219996</v>
+        <v>0.5</v>
       </c>
       <c r="AE111">
-        <v>0.0144623715219996</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="AF111">
-        <v>0.0144623715219996</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="AG111">
-        <v>0.0144623715219996</v>
+        <v>0.6</v>
       </c>
       <c r="AH111">
-        <v>0.0144623715219996</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="AI111">
-        <v>0.0144623715219996</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AJ111">
-        <v>0.0144623715219996</v>
+        <v>0.7</v>
       </c>
       <c r="AK111">
-        <v>0.0144623715219996</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="AL111">
-        <v>0.0144623715219996</v>
+        <v>0.7666666666666666</v>
       </c>
       <c r="AM111">
-        <v>0.0144623715219996</v>
+        <v>0.8</v>
       </c>
       <c r="AN111">
-        <v>0.0144623715219996</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="AO111">
-        <v>0.0144623715219996</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="AP111">
-        <v>0.0144623715219996</v>
+        <v>0.9</v>
       </c>
       <c r="AQ111">
-        <v>0.0144623715219996</v>
+        <v>0.9333333333333332</v>
       </c>
       <c r="AR111">
-        <v>0.0144623715219996</v>
+        <v>0.9666666666666668</v>
       </c>
       <c r="AS111">
-        <v>0.0144623715219996</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:45">
@@ -17150,94 +17150,94 @@
         <v>19305004.02</v>
       </c>
       <c r="P132">
-        <v>19305000</v>
+        <v>19305004.02</v>
       </c>
       <c r="Q132">
-        <v>18945254.79</v>
+        <v>19305004.02</v>
       </c>
       <c r="R132">
-        <v>18592213.38</v>
+        <v>19305004.02</v>
       </c>
       <c r="S132">
-        <v>18245750.82</v>
+        <v>19305004.02</v>
       </c>
       <c r="T132">
-        <v>17905744.53</v>
+        <v>19305004.02</v>
       </c>
       <c r="U132">
-        <v>17572074.2</v>
+        <v>19305004.02</v>
       </c>
       <c r="V132">
-        <v>17244621.76</v>
+        <v>19305004.02</v>
       </c>
       <c r="W132">
-        <v>16923271.33</v>
+        <v>19305004.02</v>
       </c>
       <c r="X132">
-        <v>16607909.21</v>
+        <v>19305004.02</v>
       </c>
       <c r="Y132">
-        <v>16298423.8</v>
+        <v>19305004.02</v>
       </c>
       <c r="Z132">
-        <v>15994705.61</v>
+        <v>19305004.02</v>
       </c>
       <c r="AA132">
-        <v>15696647.14</v>
+        <v>19305004.02</v>
       </c>
       <c r="AB132">
-        <v>15404142.94</v>
+        <v>19305004.02</v>
       </c>
       <c r="AC132">
-        <v>15117089.51</v>
+        <v>19305004.02</v>
       </c>
       <c r="AD132">
-        <v>14835385.26</v>
+        <v>19305004.02</v>
       </c>
       <c r="AE132">
-        <v>14558930.52</v>
+        <v>19305004.02</v>
       </c>
       <c r="AF132">
-        <v>14287627.47</v>
+        <v>19305004.02</v>
       </c>
       <c r="AG132">
-        <v>14021380.1</v>
+        <v>19305004.02</v>
       </c>
       <c r="AH132">
-        <v>13760094.2</v>
+        <v>19305004.02</v>
       </c>
       <c r="AI132">
-        <v>13503677.32</v>
+        <v>19305004.02</v>
       </c>
       <c r="AJ132">
-        <v>13252038.72</v>
+        <v>19305004.02</v>
       </c>
       <c r="AK132">
-        <v>13005089.36</v>
+        <v>19305004.02</v>
       </c>
       <c r="AL132">
-        <v>12762741.85</v>
+        <v>19305004.02</v>
       </c>
       <c r="AM132">
-        <v>12524910.45</v>
+        <v>19305004.02</v>
       </c>
       <c r="AN132">
-        <v>12291511</v>
+        <v>19305004.02</v>
       </c>
       <c r="AO132">
-        <v>12062460.9</v>
+        <v>19305004.02</v>
       </c>
       <c r="AP132">
-        <v>11837679.11</v>
+        <v>19305004.02</v>
       </c>
       <c r="AQ132">
-        <v>11617086.08</v>
+        <v>19305004.02</v>
       </c>
       <c r="AR132">
-        <v>11400603.77</v>
+        <v>19305004.02</v>
       </c>
       <c r="AS132">
-        <v>11188155.57</v>
+        <v>19305004.02</v>
       </c>
     </row>
     <row r="133" spans="1:45">
@@ -17272,94 +17272,94 @@
         <v>325640.846720436</v>
       </c>
       <c r="P133">
-        <v>325640.8</v>
+        <v>325640.846720436</v>
       </c>
       <c r="Q133">
-        <v>338623.564547396</v>
+        <v>325640.846720436</v>
       </c>
       <c r="R133">
-        <v>352123.930621668</v>
+        <v>325640.846720436</v>
       </c>
       <c r="S133">
-        <v>366162.53414667</v>
+        <v>325640.846720436</v>
       </c>
       <c r="T133">
-        <v>380760.833766693</v>
+        <v>325640.846720436</v>
       </c>
       <c r="U133">
-        <v>395941.143646975</v>
+        <v>325640.846720436</v>
       </c>
       <c r="V133">
-        <v>411726.667581922</v>
+        <v>325640.846720436</v>
       </c>
       <c r="W133">
-        <v>428141.534463161</v>
+        <v>325640.846720436</v>
       </c>
       <c r="X133">
-        <v>445210.835161648</v>
+        <v>325640.846720436</v>
       </c>
       <c r="Y133">
-        <v>462960.66088021</v>
+        <v>325640.846720436</v>
       </c>
       <c r="Z133">
-        <v>481418.143035132</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AA133">
-        <v>500611.494727763</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AB133">
-        <v>520570.053869524</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AC133">
-        <v>541324.328026242</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AD133">
-        <v>562906.041050353</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AE133">
-        <v>585348.181572252</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AF133">
-        <v>608685.0534249149</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AG133">
-        <v>632952.328078874</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AH133">
-        <v>658187.099167675</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AI133">
-        <v>684427.939187191</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AJ133">
-        <v>711714.958455436</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AK133">
-        <v>740089.866423008</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AL133">
-        <v>769596.035427885</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AM133">
-        <v>800278.566992018</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AN133">
-        <v>832184.360761056</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AO133">
-        <v>865362.186192592</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AP133">
-        <v>899862.757102497</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AQ133">
-        <v>935738.809183293</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AR133">
-        <v>973045.180613063</v>
+        <v>325640.846720436</v>
       </c>
       <c r="AS133">
-        <v>1011838.8958781</v>
+        <v>325640.846720436</v>
       </c>
     </row>
     <row r="134" spans="1:45">
@@ -17394,94 +17394,94 @@
         <v>207077.079356549</v>
       </c>
       <c r="P134">
-        <v>207077.1</v>
+        <v>207077.079356549</v>
       </c>
       <c r="Q134">
-        <v>209705.834654868</v>
+        <v>207077.079356549</v>
       </c>
       <c r="R134">
-        <v>212367.939710837</v>
+        <v>207077.079356549</v>
       </c>
       <c r="S134">
-        <v>215063.838787562</v>
+        <v>207077.079356549</v>
       </c>
       <c r="T134">
-        <v>217793.960882327</v>
+        <v>207077.079356549</v>
       </c>
       <c r="U134">
-        <v>220558.740438311</v>
+        <v>207077.079356549</v>
       </c>
       <c r="V134">
-        <v>223358.617413719</v>
+        <v>207077.079356549</v>
       </c>
       <c r="W134">
-        <v>226194.037351795</v>
+        <v>207077.079356549</v>
       </c>
       <c r="X134">
-        <v>229065.451451718</v>
+        <v>207077.079356549</v>
       </c>
       <c r="Y134">
-        <v>231973.316640405</v>
+        <v>207077.079356549</v>
       </c>
       <c r="Z134">
-        <v>234918.095645217</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AA134">
-        <v>237900.257067596</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AB134">
-        <v>240920.275457634</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AC134">
-        <v>243978.631389584</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AD134">
-        <v>247075.811538336</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AE134">
-        <v>250212.308756862</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AF134">
-        <v>253388.622154644</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AG134">
-        <v>256605.257177093</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AH134">
-        <v>259862.725685986</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AI134">
-        <v>263161.546040913</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AJ134">
-        <v>266502.243181768</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AK134">
-        <v>269885.348712278</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AL134">
-        <v>273311.400984602</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AM134">
-        <v>276780.945184993</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AN134">
-        <v>280294.533420558</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AO134">
-        <v>283852.724807113</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AP134">
-        <v>287456.085558153</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AQ134">
-        <v>291105.189074957</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AR134">
-        <v>294800.616037829</v>
+        <v>207077.079356549</v>
       </c>
       <c r="AS134">
-        <v>298542.954498505</v>
+        <v>207077.079356549</v>
       </c>
     </row>
     <row r="135" spans="1:45">
@@ -17516,94 +17516,94 @@
         <v>25828.1988705888</v>
       </c>
       <c r="P135">
-        <v>25828.2</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="Q135">
-        <v>25831.1278744207</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="R135">
-        <v>25834.0560807441</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="S135">
-        <v>25836.9846190078</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="T135">
-        <v>25839.9134892494</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="U135">
-        <v>25842.8426915066</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="V135">
-        <v>25845.772225817</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="W135">
-        <v>25848.7020922182</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="X135">
-        <v>25851.6322907479</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="Y135">
-        <v>25854.5628214437</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="Z135">
-        <v>25857.4936843433</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AA135">
-        <v>25860.4248794844</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AB135">
-        <v>25863.3564069045</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AC135">
-        <v>25866.2882666415</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AD135">
-        <v>25869.2204587329</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AE135">
-        <v>25872.1529832164</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AF135">
-        <v>25875.0858401297</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AG135">
-        <v>25878.0190295105</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AH135">
-        <v>25880.9525513965</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AI135">
-        <v>25883.8864058253</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AJ135">
-        <v>25886.8205928348</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AK135">
-        <v>25889.7551124624</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AL135">
-        <v>25892.6899647461</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AM135">
-        <v>25895.6251497234</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AN135">
-        <v>25898.5606674321</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AO135">
-        <v>25901.49651791</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AP135">
-        <v>25904.4327011946</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AQ135">
-        <v>25907.3692173239</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AR135">
-        <v>25910.3060663354</v>
+        <v>25828.1988705888</v>
       </c>
       <c r="AS135">
-        <v>25913.243248267</v>
+        <v>25828.1988705888</v>
       </c>
     </row>
     <row r="136" spans="1:45">
@@ -17638,94 +17638,94 @@
         <v>643748.030054217</v>
       </c>
       <c r="P136">
-        <v>643748</v>
+        <v>643748.030054217</v>
       </c>
       <c r="Q136">
-        <v>1185081.11870814</v>
+        <v>643748.030054217</v>
       </c>
       <c r="R136">
-        <v>2181625.81929349</v>
+        <v>643748.030054217</v>
       </c>
       <c r="S136">
-        <v>4016173.35747979</v>
+        <v>643748.030054217</v>
       </c>
       <c r="T136">
-        <v>7393407.38209361</v>
+        <v>643748.030054217</v>
       </c>
       <c r="U136">
-        <v>13610585.9613335</v>
+        <v>643748.030054217</v>
       </c>
       <c r="V136">
-        <v>25055842.4062374</v>
+        <v>643748.030054217</v>
       </c>
       <c r="W136">
-        <v>46125511.4562822</v>
+        <v>643748.030054217</v>
       </c>
       <c r="X136">
-        <v>84912842.7856805</v>
+        <v>643748.030054217</v>
       </c>
       <c r="Y136">
-        <v>156316767.929598</v>
+        <v>643748.030054217</v>
       </c>
       <c r="Z136">
-        <v>287764855.519318</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AA136">
-        <v>529748747.807714</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AB136">
-        <v>975218934.561667</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AC136">
-        <v>1795288755.77975</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AD136">
-        <v>3304962201.20858</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AE136">
-        <v>6084132770.42631</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AF136">
-        <v>11200331294.1488</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AG136">
-        <v>20618784275.7906</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AH136">
-        <v>37957293748.4169</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AI136">
-        <v>69875901965.53239</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AJ136">
-        <v>128635136842.45</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AK136">
-        <v>236805507550.2</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AL136">
-        <v>435937254645.981</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AM136">
-        <v>802520566156.969</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AN136">
-        <v>1477366873881.7</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AO136">
-        <v>2719697129376.83</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AP136">
-        <v>5006713367077.21</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AQ136">
-        <v>9216900834032.689</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AR136">
-        <v>16967470425411</v>
+        <v>643748.030054217</v>
       </c>
       <c r="AS136">
-        <v>31235559307979.9</v>
+        <v>643748.030054217</v>
       </c>
     </row>
     <row r="137" spans="1:45">
@@ -17760,94 +17760,94 @@
         <v>1510649.41975131</v>
       </c>
       <c r="P137">
-        <v>1510649</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="Q137">
-        <v>1535400.5418491</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="R137">
-        <v>1560557.6304691</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="S137">
-        <v>1586126.91062518</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="T137">
-        <v>1612115.13595503</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="U137">
-        <v>1638529.17075277</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="V137">
-        <v>1665375.99178192</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="W137">
-        <v>1692662.69011825</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="X137">
-        <v>1720396.47302273</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="Y137">
-        <v>1748584.6658452</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="Z137">
-        <v>1777234.71395921</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AA137">
-        <v>1806354.18472855</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AB137">
-        <v>1835950.76950609</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AC137">
-        <v>1866032.28566526</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AD137">
-        <v>1896606.67866483</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AE137">
-        <v>1927682.02414764</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AF137">
-        <v>1959266.53007354</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AG137">
-        <v>1991368.53888741</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AH137">
-        <v>2023996.52972265</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AI137">
-        <v>2057159.12064077</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AJ137">
-        <v>2090865.07090771</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AK137">
-        <v>2125123.28330741</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AL137">
-        <v>2159942.80649333</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AM137">
-        <v>2195332.83737846</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AN137">
-        <v>2231302.72356452</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AO137">
-        <v>2267861.96581094</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AP137">
-        <v>2305020.22054435</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AQ137">
-        <v>2342787.30240905</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AR137">
-        <v>2381173.18685946</v>
+        <v>1510649.41975131</v>
       </c>
       <c r="AS137">
-        <v>2420188.01279487</v>
+        <v>1510649.41975131</v>
       </c>
     </row>
     <row r="138" spans="1:45">
@@ -17882,94 +17882,94 @@
         <v>682291.1157233421</v>
       </c>
       <c r="P138">
-        <v>682291.1</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="Q138">
-        <v>675510.049196484</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="R138">
-        <v>668796.392867261</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="S138">
-        <v>662149.461202402</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="T138">
-        <v>655568.591048982</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="U138">
-        <v>649053.125844917</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="V138">
-        <v>642602.415553466</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="W138">
-        <v>636215.816598372</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="X138">
-        <v>629892.691799654</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="Y138">
-        <v>623632.410310042</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="Z138">
-        <v>617434.347552032</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AA138">
-        <v>611297.885155577</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AB138">
-        <v>605222.41089639</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AC138">
-        <v>599207.318634868</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AD138">
-        <v>593252.0082556159</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AE138">
-        <v>587355.885607571</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AF138">
-        <v>581518.3624447311</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AG138">
-        <v>575738.8563674639</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AH138">
-        <v>570016.790764401</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AI138">
-        <v>564351.594754911</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AJ138">
-        <v>558742.703132143</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AK138">
-        <v>553189.556306642</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AL138">
-        <v>547691.60025051</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AM138">
-        <v>542248.28644214</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AN138">
-        <v>536859.071811488</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AO138">
-        <v>531523.41868589</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AP138">
-        <v>526240.794736424</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AQ138">
-        <v>521010.672924795</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AR138">
-        <v>515832.531450756</v>
+        <v>682291.1157233421</v>
       </c>
       <c r="AS138">
-        <v>510705.853700051</v>
+        <v>682291.1157233421</v>
       </c>
     </row>
     <row r="139" spans="1:45">
@@ -18004,94 +18004,94 @@
         <v>643314.319559388</v>
       </c>
       <c r="P139">
-        <v>643314.3</v>
+        <v>643314.319559388</v>
       </c>
       <c r="Q139">
-        <v>645100.341854176</v>
+        <v>643314.319559388</v>
       </c>
       <c r="R139">
-        <v>646891.34231957</v>
+        <v>643314.319559388</v>
       </c>
       <c r="S139">
-        <v>648687.315162839</v>
+        <v>643314.319559388</v>
       </c>
       <c r="T139">
-        <v>650488.274188861</v>
+        <v>643314.319559388</v>
       </c>
       <c r="U139">
-        <v>652294.233240839</v>
+        <v>643314.319559388</v>
       </c>
       <c r="V139">
-        <v>654105.206200411</v>
+        <v>643314.319559388</v>
       </c>
       <c r="W139">
-        <v>655921.206987753</v>
+        <v>643314.319559388</v>
       </c>
       <c r="X139">
-        <v>657742.249561689</v>
+        <v>643314.319559388</v>
       </c>
       <c r="Y139">
-        <v>659568.347919796</v>
+        <v>643314.319559388</v>
       </c>
       <c r="Z139">
-        <v>661399.516098514</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AA139">
-        <v>663235.768173252</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AB139">
-        <v>665077.118258497</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AC139">
-        <v>666923.58050792</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AD139">
-        <v>668775.169114491</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AE139">
-        <v>670631.898310581</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AF139">
-        <v>672493.782368075</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AG139">
-        <v>674360.835598483</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AH139">
-        <v>676233.072353046</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AI139">
-        <v>678110.50702285</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AJ139">
-        <v>679993.154038934</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AK139">
-        <v>681881.027872403</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AL139">
-        <v>683774.143034538</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AM139">
-        <v>685672.5140769091</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AN139">
-        <v>687576.155591484</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AO139">
-        <v>689485.0822107421</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AP139">
-        <v>691399.30860779</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AQ139">
-        <v>693318.849496469</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AR139">
-        <v>695243.719631471</v>
+        <v>643314.319559388</v>
       </c>
       <c r="AS139">
-        <v>697173.933808452</v>
+        <v>643314.319559388</v>
       </c>
     </row>
     <row r="140" spans="1:45">
@@ -18126,94 +18126,94 @@
         <v>297565.165626813</v>
       </c>
       <c r="P140">
-        <v>297565.2</v>
+        <v>297565.165626813</v>
       </c>
       <c r="Q140">
-        <v>302802.311395585</v>
+        <v>297565.165626813</v>
       </c>
       <c r="R140">
-        <v>308131.595315946</v>
+        <v>297565.165626813</v>
       </c>
       <c r="S140">
-        <v>313554.673986331</v>
+        <v>297565.165626813</v>
       </c>
       <c r="T140">
-        <v>319073.198182953</v>
+        <v>297565.165626813</v>
       </c>
       <c r="U140">
-        <v>324688.847735487</v>
+        <v>297565.165626813</v>
       </c>
       <c r="V140">
-        <v>330403.332038406</v>
+        <v>297565.165626813</v>
       </c>
       <c r="W140">
-        <v>336218.390571317</v>
+        <v>297565.165626813</v>
       </c>
       <c r="X140">
-        <v>342135.79342846</v>
+        <v>297565.165626813</v>
       </c>
       <c r="Y140">
-        <v>348157.341857515</v>
+        <v>297565.165626813</v>
       </c>
       <c r="Z140">
-        <v>354284.868807906</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AA140">
-        <v>360520.239488742</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AB140">
-        <v>366865.351936587</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AC140">
-        <v>373322.137593217</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AD140">
-        <v>379892.56189355</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AE140">
-        <v>386578.62486392</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AF140">
-        <v>393382.36173088</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AG140">
-        <v>400305.843540725</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AH140">
-        <v>407351.177789912</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AI140">
-        <v>414520.509066581</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AJ140">
-        <v>421816.019703363</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AK140">
-        <v>429239.930441678</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AL140">
-        <v>436794.501107724</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AM140">
-        <v>444482.031300367</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AN140">
-        <v>452304.861091135</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AO140">
-        <v>460265.371736529</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AP140">
-        <v>468365.986402876</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AQ140">
-        <v>476609.170903936</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AR140">
-        <v>484997.434451492</v>
+        <v>297565.165626813</v>
       </c>
       <c r="AS140">
-        <v>493533.330419149</v>
+        <v>297565.165626813</v>
       </c>
     </row>
     <row r="141" spans="1:45">
@@ -18980,94 +18980,94 @@
         <v>62605.7129653388</v>
       </c>
       <c r="P147">
-        <v>62605.71</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="Q147">
-        <v>64412.6003167653</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="R147">
-        <v>66271.64007192561</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="S147">
-        <v>68184.3343728467</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="T147">
-        <v>70152.2317664452</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="U147">
-        <v>72176.9254929162</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="V147">
-        <v>74260.0547756453</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="W147">
-        <v>76403.3061483487</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="X147">
-        <v>78608.41482051789</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="Y147">
-        <v>80877.1660822712</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="Z147">
-        <v>83211.3967497531</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AA147">
-        <v>85612.9966522483</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AB147">
-        <v>88083.91016221741</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AC147">
-        <v>90626.13776949049</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AD147">
-        <v>93241.7377008951</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AE147">
-        <v>95932.8275866278</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AF147">
-        <v>98701.58617472131</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AG147">
-        <v>101550.255094992</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AH147">
-        <v>104481.140673898</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AI147">
-        <v>107496.615801778</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AJ147">
-        <v>110599.121853978</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AK147">
-        <v>113791.170667428</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AL147">
-        <v>117075.346574264</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AM147">
-        <v>120454.308494143</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AN147">
-        <v>123930.792086945</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AO147">
-        <v>127507.611967607</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AP147">
-        <v>131187.663984877</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AQ147">
-        <v>134973.92756584</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AR147">
-        <v>138869.468128107</v>
+        <v>62605.7129653388</v>
       </c>
       <c r="AS147">
-        <v>142877.439561624</v>
+        <v>62605.7129653388</v>
       </c>
     </row>
     <row r="148" spans="1:45">
@@ -19102,94 +19102,94 @@
         <v>461339.584568216</v>
       </c>
       <c r="P148">
-        <v>461339.6</v>
+        <v>461339.584568216</v>
       </c>
       <c r="Q148">
-        <v>467291.089319365</v>
+        <v>461339.584568216</v>
       </c>
       <c r="R148">
-        <v>473319.355540428</v>
+        <v>461339.584568216</v>
       </c>
       <c r="S148">
-        <v>479425.389119917</v>
+        <v>461339.584568216</v>
       </c>
       <c r="T148">
-        <v>485610.193291897</v>
+        <v>461339.584568216</v>
       </c>
       <c r="U148">
-        <v>491874.784232609</v>
+        <v>461339.584568216</v>
       </c>
       <c r="V148">
-        <v>498220.191227424</v>
+        <v>461339.584568216</v>
       </c>
       <c r="W148">
-        <v>504647.456839962</v>
+        <v>461339.584568216</v>
       </c>
       <c r="X148">
-        <v>511157.637083384</v>
+        <v>461339.584568216</v>
       </c>
       <c r="Y148">
-        <v>517751.801593896</v>
+        <v>461339.584568216</v>
       </c>
       <c r="Z148">
-        <v>524431.033806496</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AA148">
-        <v>531196.431132984</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AB148">
-        <v>538049.105142267</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AC148">
-        <v>544990.181742992</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AD148">
-        <v>552020.80136854</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AE148">
-        <v>559142.119164395</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AF148">
-        <v>566355.305177939</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AG148">
-        <v>573661.544550697</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AH148">
-        <v>581062.0377130531</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AI148">
-        <v>588558.000581486</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AJ148">
-        <v>596150.664758348</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AK148">
-        <v>603841.277734216</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AL148">
-        <v>611631.10309286</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AM148">
-        <v>619521.4207188539</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AN148">
-        <v>627513.527007857</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AO148">
-        <v>635608.735079621</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AP148">
-        <v>643808.374993736</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AQ148">
-        <v>652113.7939681601</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AR148">
-        <v>660526.356600572</v>
+        <v>461339.584568216</v>
       </c>
       <c r="AS148">
-        <v>669047.44509258</v>
+        <v>461339.584568216</v>
       </c>
     </row>
     <row r="149" spans="1:45">

</xml_diff>